<commit_message>
Buiilt sample test case
</commit_message>
<xml_diff>
--- a/src/test/resources/apps/toyota/dataProviders/ChangeZipCode.xlsx
+++ b/src/test/resources/apps/toyota/dataProviders/ChangeZipCode.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TestScenario</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>ZipCode</t>
+  </si>
+  <si>
+    <t>92055</t>
   </si>
 </sst>
 </file>
@@ -507,8 +510,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -854,7 +858,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,8 +879,8 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>92055</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>